<commit_message>
add ideal case from hantao-REGCV2
</commit_message>
<xml_diff>
--- a/bshe/Test_ieee14_vsg/ieee14_vsg_twoInv.xlsx
+++ b/bshe/Test_ieee14_vsg/ieee14_vsg_twoInv.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ACE" sheetId="11" r:id="rId11"/>
     <sheet name="ACEc" sheetId="12" r:id="rId12"/>
     <sheet name="COI" sheetId="13" r:id="rId13"/>
-    <sheet name="REGCV1" sheetId="14" r:id="rId14"/>
+    <sheet name="REGCV2" sheetId="14" r:id="rId14"/>
     <sheet name="GENROU" sheetId="15" r:id="rId15"/>
     <sheet name="TGOV1N" sheetId="16" r:id="rId16"/>
     <sheet name="EXST1" sheetId="17" r:id="rId17"/>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="str">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="Y2" t="str">
         <v>1</v>
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="str">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="Y3" t="str">
         <v>1</v>

</xml_diff>